<commit_message>
funcao SE exercicio finalizado pt2
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/6.Funcoes_Mercado/1.SE/2.Funcao_SE_Exercicios.xlsx
+++ b/2.Excel/hands-on/6.Funcoes_Mercado/1.SE/2.Funcao_SE_Exercicios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\6.Funcoes_Mercado\1.SE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF426C2-ABE2-4443-BC86-356322C0AAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D34F358-C87F-4782-BED4-C35514161260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="957" xr2:uid="{85B08948-7BCF-4007-BABB-111144F4B1B5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="957" activeTab="1" xr2:uid="{85B08948-7BCF-4007-BABB-111144F4B1B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercicio1" sheetId="3" r:id="rId1"/>
@@ -2575,7 +2575,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
         <top style="thin">
@@ -2601,6 +2601,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.79998168889431442"/>
@@ -2608,7 +2609,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
         <top style="thin">
@@ -2725,8 +2726,12 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D801CA54-D910-4E4A-BDC6-FA3B03D4D0B9}" name="Vendedor" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{A4CB21AD-F60D-4EA3-8242-0EB9FD4F29A3}" name="Faturado" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{BBAE7579-7F82-4A56-B2BB-76B78C389B28}" name="Bônus" dataDxfId="1" dataCellStyle="Porcentagem"/>
-    <tableColumn id="4" xr3:uid="{4B10A2AF-FE30-4EDA-9D5D-54934374247A}" name="Salário" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{BBAE7579-7F82-4A56-B2BB-76B78C389B28}" name="Bônus" dataDxfId="1" dataCellStyle="Porcentagem">
+      <calculatedColumnFormula>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{4B10A2AF-FE30-4EDA-9D5D-54934374247A}" name="Salário" dataDxfId="0">
+      <calculatedColumnFormula>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3031,7 +3036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609AF048-41B8-465E-8ECB-BABA18201A44}">
   <dimension ref="A1:H401"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -9095,8 +9100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2832FA5D-9351-41D3-8C94-970B4E969281}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9133,8 +9138,14 @@
       <c r="B2" s="20">
         <v>58729</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="20"/>
+      <c r="C2" s="25">
+        <f>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</f>
+        <v>0.05</v>
+      </c>
+      <c r="D2" s="20">
+        <f>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</f>
+        <v>2936.4500000000003</v>
+      </c>
       <c r="G2" s="16" t="s">
         <v>328</v>
       </c>
@@ -9152,8 +9163,14 @@
       <c r="B3" s="21">
         <v>162517</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="21"/>
+      <c r="C3" s="26">
+        <f>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</f>
+        <v>0.1</v>
+      </c>
+      <c r="D3" s="21">
+        <f>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</f>
+        <v>16251.7</v>
+      </c>
       <c r="G3" s="17">
         <v>0</v>
       </c>
@@ -9171,8 +9188,14 @@
       <c r="B4" s="20">
         <v>432944</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="20"/>
+      <c r="C4" s="25">
+        <f>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</f>
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="20">
+        <f>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</f>
+        <v>129883.2</v>
+      </c>
       <c r="G4" s="17">
         <v>50001</v>
       </c>
@@ -9190,8 +9213,14 @@
       <c r="B5" s="21">
         <v>514342</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="21"/>
+      <c r="C5" s="26">
+        <f>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</f>
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="21">
+        <f>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</f>
+        <v>154302.6</v>
+      </c>
       <c r="G5" s="17">
         <v>100001</v>
       </c>
@@ -9209,8 +9238,14 @@
       <c r="B6" s="20">
         <v>214635</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="20"/>
+      <c r="C6" s="25">
+        <f>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</f>
+        <v>0.15</v>
+      </c>
+      <c r="D6" s="20">
+        <f>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</f>
+        <v>32195.25</v>
+      </c>
       <c r="G6" s="17">
         <v>200001</v>
       </c>
@@ -9228,8 +9263,14 @@
       <c r="B7" s="21">
         <v>239239</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="21"/>
+      <c r="C7" s="26">
+        <f>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</f>
+        <v>0.15</v>
+      </c>
+      <c r="D7" s="21">
+        <f>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</f>
+        <v>35885.85</v>
+      </c>
       <c r="G7" s="17">
         <v>300001</v>
       </c>
@@ -9247,8 +9288,14 @@
       <c r="B8" s="20">
         <v>40622</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="20"/>
+      <c r="C8" s="25">
+        <f>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</f>
+        <v>0.02</v>
+      </c>
+      <c r="D8" s="20">
+        <f>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</f>
+        <v>812.44</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
@@ -9257,8 +9304,14 @@
       <c r="B9" s="21">
         <v>389479</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="21"/>
+      <c r="C9" s="26">
+        <f>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</f>
+        <v>0.3</v>
+      </c>
+      <c r="D9" s="21">
+        <f>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</f>
+        <v>116843.7</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
@@ -9267,8 +9320,14 @@
       <c r="B10" s="20">
         <v>553835</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="20"/>
+      <c r="C10" s="25">
+        <f>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</f>
+        <v>0.3</v>
+      </c>
+      <c r="D10" s="20">
+        <f>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</f>
+        <v>166150.5</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
@@ -9277,8 +9336,14 @@
       <c r="B11" s="21">
         <v>446282</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="21"/>
+      <c r="C11" s="26">
+        <f>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</f>
+        <v>0.3</v>
+      </c>
+      <c r="D11" s="21">
+        <f>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</f>
+        <v>133884.6</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
@@ -9287,8 +9352,14 @@
       <c r="B12" s="20">
         <v>310454</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="20"/>
+      <c r="C12" s="25">
+        <f>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</f>
+        <v>0.3</v>
+      </c>
+      <c r="D12" s="20">
+        <f>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</f>
+        <v>93136.2</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
@@ -9297,8 +9368,14 @@
       <c r="B13" s="21">
         <v>523471</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="21"/>
+      <c r="C13" s="26">
+        <f>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</f>
+        <v>0.3</v>
+      </c>
+      <c r="D13" s="21">
+        <f>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</f>
+        <v>157041.29999999999</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
@@ -9307,8 +9384,14 @@
       <c r="B14" s="20">
         <v>54717</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="20"/>
+      <c r="C14" s="25">
+        <f>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</f>
+        <v>0.05</v>
+      </c>
+      <c r="D14" s="20">
+        <f>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</f>
+        <v>2735.8500000000004</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
@@ -9317,8 +9400,14 @@
       <c r="B15" s="21">
         <v>398008</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="21"/>
+      <c r="C15" s="26">
+        <f>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</f>
+        <v>0.3</v>
+      </c>
+      <c r="D15" s="21">
+        <f>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</f>
+        <v>119402.4</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
@@ -9327,8 +9416,14 @@
       <c r="B16" s="20">
         <v>70346</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="20"/>
+      <c r="C16" s="25">
+        <f>IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$3,$I$3,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$4,$I$4,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$5,$I$5,IF(Tabela2[[#This Row],[Faturado]]&lt;=$H$6,$I$6,$I$7))))</f>
+        <v>0.05</v>
+      </c>
+      <c r="D16" s="20">
+        <f>Tabela2[[#This Row],[Faturado]]*Tabela2[[#This Row],[Bônus]]</f>
+        <v>3517.3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>